<commit_message>
update for new blokcs design
</commit_message>
<xml_diff>
--- a/12345upload.xlsx
+++ b/12345upload.xlsx
@@ -1,99 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
-  <si>
-    <t>ID card/Номер ID карты*</t>
-  </si>
-  <si>
-    <t>IIN/ИИН**</t>
-  </si>
-  <si>
-    <t>Lastname/Фамилия***</t>
-  </si>
-  <si>
-    <t>Firstname/Имя***</t>
-  </si>
-  <si>
-    <t>Complex/Комплекс*</t>
-  </si>
-  <si>
-    <t>Bulding (Block)/Блок*</t>
-  </si>
-  <si>
-    <t>Object number/Номер объекта*</t>
-  </si>
-  <si>
-    <t>Place number/Номер места*</t>
-  </si>
-  <si>
-    <t>Start date/Дата заселения*</t>
-  </si>
-  <si>
-    <t>End date/Дата выселения*</t>
-  </si>
-  <si>
-    <t>Comment/Комментарий</t>
-  </si>
-  <si>
-    <t>Reasons for accomodation/Основание заселения</t>
-  </si>
-  <si>
-    <t>Type of accomodation/Тип заселения*</t>
-  </si>
-  <si>
-    <t>Number of the agreement/Номер договора</t>
-  </si>
-  <si>
-    <t>Date of the agreement/Дата договора</t>
-  </si>
-  <si>
-    <t>Cost of living/Стоимость проживания</t>
-  </si>
-  <si>
-    <t>Discount/Скидка</t>
-  </si>
-  <si>
-    <t>Блок 27</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -108,35 +46,93 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -424,84 +420,404 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:Q10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:17">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ID card/Номер ID карты*</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>IIN/ИИН**</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Lastname/Фамилия***</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Firstname/Имя***</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Complex/Комплекс*</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Bulding (Block)/Блок*</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Object number/Номер объекта*</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Place number/Номер места*</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Start date/Дата заселения*</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>End date/Дата выселения*</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Comment/Комментарий</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Reasons for accomodation/Основание заселения</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Type of accomodation/Тип заселения*</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Number of the agreement/Номер договора</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Date of the agreement/Дата договора</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Cost of living/Стоимость проживания</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Discount/Скидка</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>202031974</v>
+      </c>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Блок 23</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Блок 23</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>1111</v>
+      </c>
+      <c r="H2" t="n">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
+      <c r="Q2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>202015678</v>
+      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Блок 23</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Блок 23</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>1111</v>
+      </c>
+      <c r="H3" t="n">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17">
-      <c r="A2">
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
+      <c r="Q3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
         <v>202107823</v>
       </c>
-      <c r="E2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2">
-        <v>903</v>
-      </c>
-      <c r="H2">
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Блок 25</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Блок 25</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>409</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr"/>
+      <c r="Q4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>201922256</v>
+      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Блок 25</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Блок 25</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>409</v>
+      </c>
+      <c r="H5" t="n">
         <v>2</v>
       </c>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr"/>
+      <c r="Q5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>202021479</v>
+      </c>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Блок 25</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Блок 25</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>517</v>
+      </c>
+      <c r="H6" t="n">
+        <v>1</v>
+      </c>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
+      <c r="P6" t="inlineStr"/>
+      <c r="Q6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>202021013</v>
+      </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Блок 25</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Блок 25</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>517</v>
+      </c>
+      <c r="H7" t="n">
+        <v>2</v>
+      </c>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
+      <c r="P7" t="inlineStr"/>
+      <c r="Q7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>202121134</v>
+      </c>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Блок 26</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Блок 26</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>204</v>
+      </c>
+      <c r="H8" t="n">
+        <v>1</v>
+      </c>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr"/>
+      <c r="P8" t="inlineStr"/>
+      <c r="Q8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>202013756</v>
+      </c>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Блок 26</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Блок 26</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>204</v>
+      </c>
+      <c r="H9" t="n">
+        <v>2</v>
+      </c>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
+      <c r="P9" t="inlineStr"/>
+      <c r="Q9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>202031123</v>
+      </c>
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Блок 26</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Блок 26</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>327</v>
+      </c>
+      <c r="H10" t="n">
+        <v>1</v>
+      </c>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
+      <c r="P10" t="inlineStr"/>
+      <c r="Q10" t="inlineStr"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>